<commit_message>
made changes to recmodal.html and added a .csv to the project
</commit_message>
<xml_diff>
--- a/worksheets/Clexan foods.xlsx
+++ b/worksheets/Clexan foods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Clarkstore\worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8F48F6-6CBC-4A3E-95F0-9BC9D143ECCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386D01A0-B55A-4B77-913D-604FBD6B6275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{334EE45C-64B1-45AE-96E3-202C83F441C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{334EE45C-64B1-45AE-96E3-202C83F441C2}"/>
   </bookViews>
   <sheets>
     <sheet name="product_sheet" sheetId="2" r:id="rId1"/>

</xml_diff>